<commit_message>
Updated adj adn target tests, updates layout spreadsheet with tests identified
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliff\Documents\mines\Spring2016\306\ClueLayout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliff\Documents\mines\Spring2016\306\ClueBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="30">
   <si>
     <t>X</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>DR</t>
+  </si>
+  <si>
+    <t>Number of Doors: 17</t>
+  </si>
+  <si>
+    <t>Purple: adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Orange: adjacency tests, room exits</t>
+  </si>
+  <si>
+    <t>White: adjacency tests beside room entrance</t>
+  </si>
+  <si>
+    <t>Blue: various walkway scenarios</t>
+  </si>
+  <si>
+    <t>Pink: target tests</t>
+  </si>
+  <si>
+    <t>Light Green: door direction tests (in BoarsTest)</t>
   </si>
 </sst>
 </file>
@@ -108,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +160,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,12 +226,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -449,15 +529,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -467,7 +547,7 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -518,14 +598,14 @@
       <c r="T1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="V1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -550,7 +630,7 @@
       <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -593,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -661,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -698,10 +778,10 @@
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -728,8 +808,11 @@
       <c r="V4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -796,8 +879,11 @@
       <c r="V5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -810,13 +896,13 @@
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -831,10 +917,10 @@
       <c r="K6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="11" t="s">
         <v>3</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -864,9 +950,12 @@
       <c r="V6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="Y6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -875,7 +964,7 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -908,7 +997,7 @@
       <c r="N7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="11" t="s">
         <v>3</v>
       </c>
       <c r="P7" s="2" t="s">
@@ -932,12 +1021,15 @@
       <c r="V7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="Y7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -952,7 +1044,7 @@
       <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -967,7 +1059,7 @@
       <c r="K8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M8" s="3" t="s">
@@ -985,7 +1077,7 @@
       <c r="Q8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="S8" s="2" t="s">
@@ -1000,8 +1092,11 @@
       <c r="V8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1014,7 +1109,7 @@
       <c r="D9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1056,21 +1151,24 @@
       <c r="R9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="U9" s="11" t="s">
         <v>3</v>
       </c>
       <c r="V9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="Y9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1082,7 +1180,7 @@
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1136,8 +1234,11 @@
       <c r="V10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1316,7 @@
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1248,7 +1349,7 @@
       <c r="N12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P12" s="2" t="s">
@@ -1273,7 +1374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1341,7 +1442,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1357,10 +1458,10 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1384,7 +1485,7 @@
       <c r="N14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="P14" s="2" t="s">
@@ -1409,7 +1510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1477,7 +1578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1615,7 @@
       <c r="L16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="10" t="s">
         <v>3</v>
       </c>
       <c r="N16" s="3" t="s">
@@ -1635,7 +1736,7 @@
       <c r="G18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="9" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="4" t="s">
@@ -1685,7 +1786,7 @@
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1771,7 +1872,7 @@
       <c r="G20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="10" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -1810,7 +1911,7 @@
       <c r="T20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="U20" s="10" t="s">
         <v>3</v>
       </c>
       <c r="V20" s="1">
@@ -1882,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="V21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -1950,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="V22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -2018,7 +2119,7 @@
         <v>2</v>
       </c>
       <c r="V23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2040,7 +2141,7 @@
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -2086,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="V24" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -2108,7 +2209,7 @@
       <c r="F25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -2135,7 +2236,7 @@
       <c r="O25" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="P25" s="11" t="s">
         <v>3</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -2154,7 +2255,7 @@
         <v>2</v>
       </c>
       <c r="V25" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>